<commit_message>
added stock adjustment methods
</commit_message>
<xml_diff>
--- a/utils/GuidedKarobarData.xlsx
+++ b/utils/GuidedKarobarData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\VisualStudioProjects\Karobar_Revamp_Selenium\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C827FC4-EEEB-4547-8D07-15328669CA9D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99863323-7A68-4BBB-971B-1B7312ED70F6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" firstSheet="9" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Overview" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="221">
   <si>
     <t>Total To Receive</t>
   </si>
@@ -614,10 +614,6 @@
   </si>
   <si>
     <t>off by a 0.01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Party 17
-</t>
   </si>
   <si>
     <t>Billing Items:
@@ -666,20 +662,6 @@
     <t>Cash Sale Return</t>
   </si>
   <si>
-    <t xml:space="preserve">Billing Items:
-Item 4:  
-22.40 PCS @ Rs. 369.50  
-Item 5:  
-4.25 @ Rs. 3561.77  
-Item 7:  
-6.50 JAR @ Rs. 656.45  
-Item 13:  
-7.75 CASE @ Rs. 875.75  
-Item 19:  
-2.80 @ Rs. 4555.45  
-Charge 1: Rs. 500.75  </t>
-  </si>
-  <si>
     <t>of by 0.03
 &lt;&lt;(2837.94) app</t>
   </si>
@@ -689,17 +671,6 @@
   </si>
   <si>
     <t>Cash Purchase Return</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Billing Items:
-Item 6:  
-9.75 CAN @ Rs. 369.50  
-Item 8:  
-15.45 KG @ Rs. 986.99  
-Item 10:  
-8.25 BOX @ Rs. 986.30  
-Tax: 13%  
-Charge 1: Rs. 400.50  </t>
   </si>
   <si>
     <t>&lt;&lt;(30897.59) App</t>
@@ -713,20 +684,6 @@
 Item 17:  
 5.50 BTL @ Rs. 458.56  
 Tax: 13%  </t>
-  </si>
-  <si>
-    <t>Quotation No.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Billing Items
-Item 6:  
-9.75 CAN @ Rs. 369.50  
-Item 8:  
-15.45 KG @ Rs. 986.99  with 6.6% Discount
-Item 10:  
-8.25 BOX @ Rs. 986.30  
-Tax: 13%  
-</t>
   </si>
   <si>
     <t>off by 0.03</t>
@@ -867,19 +824,6 @@
   <si>
     <t xml:space="preserve">Billing Items:
 Item 3:  
-6.25 BOX @ Rs. 880.99  
-Item 6:  
-12.10 CAN @ Rs. 369.75  
-Item 8:  
-9.85 KG @ Rs. 986.99  
-Item 12:  
-18.20 BOX @ Rs. 980.25  
-Overall Discount: 8.75%  
-Tax: 13%  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Billing Items:
-Item 3:  
 8.10 BOX @ Rs. 880.25  
 Item 8:  
 11.35 KG @ Rs. 986.60  
@@ -891,56 +835,6 @@
 3.75 @ Rs. 4555.75  
 Overall Discount: 9.75%  
 Tax: 13%  </t>
-  </si>
-  <si>
-    <t>Billing Items:
-Item 2:
-69 @ Rs. 1107.88 
-Item 8:
-71.66 KG @ Rs. Rs. 873.87
-Item 17:
-33.33 BTL @ Rs. 11.11 with 3.3% Discount
-Item 20:
-12.88 DZN @ Rs. 49.07
-Overall Discount: Rs. 1200.33
-Charge 1: Rs. 1700.99
-Charge 2: Rs. 2200.11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Billing Items
-Item 1:  
-7.30 @ Rs. 650.45  
-Item 4:  
-18.40 PCS @ Rs. 369.99  
-Item 14:  
-5.50 BAGS @ Rs. 458.99  
-Item 20:  
-6.85 BOX @ Rs. 955.99  
-Overall Discount: 10.50%  
-Tax: 13%  
-Charge 1: Rs. 350.75  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Billing Items
-Item 8:  
-18.25 KG @ Rs. 986.99  
-Item 9:  
-5.75 @ Rs. 650.50  
-Item 12:  
-10.20 BOX @ Rs. 980.25  
-Item 13:  
-8.10 CASE @ Rs. 875.99  with 9% Discount
-Item 15:  
-6.50 BOR @ Rs. 788.45  
-Item 16:  
-3.85 @ Rs. 3636.69  
-Item 19:  
-2.90 @ Rs. 4555.75 with 8.8% Discount  
-Overall Discount: 9.50%  
-Tax: 13%  
-Charge 1: Rs. 450.25
-Charge 2: Rs. 866.99  
-</t>
   </si>
   <si>
     <t>Billing Items:
@@ -1026,6 +920,109 @@
 Item 12:  
 12.30 PCS@ Rs. 90.25  
 Tax: 13%  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Party 17
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Billing Items:
+Item 6:  
+9.75 CAN @ Rs. 369.50  
+Item 8:  
+15.45 KG @ Rs. 986.99  with 6.6% Discount
+Item 10:  
+8.25 BOX @ Rs. 986.30  
+Tax: 13%  
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Billing Items:
+Item 1:  
+7.30 @ Rs. 650.45  
+Item 4:  
+18.40 PCS @ Rs. 369.99  
+Item 14:  
+5.50 BAGS @ Rs. 458.99  
+Item 20:  
+6.85 BOX @ Rs. 955.99  
+Overall Discount: 10.50%  
+Tax: 13%  
+Charge 1: Rs. 350.75  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Billing Items:
+Item 8:  
+18.25 KG @ Rs. 986.99  
+Item 9:  
+5.75 @ Rs. 650.50  
+Item 12:  
+10.20 BOX @ Rs. 980.25  
+Item 13:  
+8.10 CASE @ Rs. 875.99  with 9% Discount
+Item 15:  
+6.50 BOR @ Rs. 788.45  
+Item 16:  
+3.85 @ Rs. 3636.69  
+Item 19:  
+2.90 @ Rs. 4555.75 with 8.8% Discount  
+Overall Discount: 9.50%  
+Tax: 13%  
+Charge 1: Rs. 450.25
+Charge 2: Rs. 866.99  
+</t>
+  </si>
+  <si>
+    <t>Billing Items:
+Item 2:
+69 @ Rs. 1107.88 
+Item 8:
+71.66 KG @ Rs. 873.87
+Item 17:
+33.33 BTL @ Rs. 11.11 with 3.3% Discount
+Item 20:
+12.88 DZN @ Rs. 49.07
+Overall Discount: Rs. 1200.33
+Charge 1: Rs. 1700.99
+Charge 2: Rs. 2200.11</t>
+  </si>
+  <si>
+    <t>Billing Items:
+Item 6:  
+9.75 CAN @ Rs. 369.50
+Item 8:  
+15.45 KG @ Rs. 986.99
+Item 10:  
+8.25 BOX @ Rs. 986.30
+Tax: 13%  
+Charge 1: Rs. 400.50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Billing Items:
+Item 3:  
+6.25 BOX @ Rs. 880.99  
+Item 6:  
+12.10 CAN @ Rs. 369.75  
+Item 8:
+9.85 KG @ Rs. 986.99  
+Item 12:  
+18.20 BOX @ Rs. 980.25  
+Overall Discount: 8.75%  
+Tax: 13%  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Billing Items:
+Item 4:  
+22.40 PCS @ Rs. 369.50  
+Item 5:
+4.25 @ Rs. 3561.77  
+Item 7:  
+6.50 JAR @ Rs. 656.45  
+Item 13:  
+7.75 CASE @ Rs. 875.75  
+Item 19:  
+2.80 @ Rs. 4555.45  
+Charge 1: Rs. 500.75  </t>
   </si>
 </sst>
 </file>
@@ -1129,7 +1126,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -1163,19 +1160,22 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1483,28 +1483,28 @@
       <c r="J6" s="6"/>
     </row>
     <row r="12" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
-      <c r="F12" s="18" t="s">
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
+      <c r="F12" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="G12" s="19"/>
+      <c r="G12" s="22"/>
       <c r="H12" s="9"/>
-      <c r="J12" s="18" t="s">
+      <c r="J12" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="K12" s="19"/>
-      <c r="M12" s="18" t="s">
+      <c r="K12" s="22"/>
+      <c r="M12" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="N12" s="19"/>
-      <c r="P12" s="18" t="s">
+      <c r="N12" s="22"/>
+      <c r="P12" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="Q12" s="19"/>
+      <c r="Q12" s="22"/>
     </row>
     <row r="13" spans="2:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B13" s="3" t="s">
@@ -2234,15 +2234,15 @@
   </sheetPr>
   <dimension ref="A1:AC20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.7109375" customWidth="1"/>
     <col min="2" max="2" width="18.42578125" customWidth="1"/>
-    <col min="3" max="3" width="48.140625" style="21" customWidth="1"/>
+    <col min="3" max="3" width="48.140625" style="18" customWidth="1"/>
     <col min="4" max="6" width="20.140625" customWidth="1"/>
     <col min="7" max="7" width="16.28515625" customWidth="1"/>
     <col min="8" max="8" width="30" customWidth="1"/>
@@ -2257,7 +2257,7 @@
         <v>178</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>166</v>
@@ -2306,7 +2306,7 @@
         <v>179</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="D2" s="13">
         <v>2670</v>
@@ -2390,7 +2390,7 @@
         <v>53</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D4" s="13">
         <v>38510.400000000001</v>
@@ -2433,7 +2433,7 @@
         <v>46</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D5" s="13">
         <v>1928.92</v>
@@ -2476,7 +2476,7 @@
         <v>77</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D6" s="13">
         <v>18023.169999999998</v>
@@ -2562,7 +2562,7 @@
         <v>75</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="D8" s="13">
         <v>565320.32999999996</v>
@@ -2607,7 +2607,7 @@
         <v>59</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="D9" s="13">
         <v>125453.23</v>
@@ -2652,7 +2652,7 @@
         <v>179</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="D10" s="13">
         <v>77212</v>
@@ -2696,8 +2696,8 @@
       <c r="B11" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="20" t="s">
-        <v>203</v>
+      <c r="C11" s="17" t="s">
+        <v>198</v>
       </c>
       <c r="D11" s="13">
         <v>28846.5</v>
@@ -2735,22 +2735,22 @@
       <c r="AC11" s="12"/>
     </row>
     <row r="13" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C13" s="20"/>
+      <c r="C13" s="17"/>
     </row>
     <row r="14" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C14" s="20"/>
+      <c r="C14" s="17"/>
     </row>
     <row r="16" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C16" s="20"/>
+      <c r="C16" s="17"/>
     </row>
     <row r="17" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C17" s="20"/>
+      <c r="C17" s="17"/>
     </row>
     <row r="19" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C19" s="20"/>
+      <c r="C19" s="17"/>
     </row>
     <row r="20" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C20" s="20"/>
+      <c r="C20" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2766,7 +2766,7 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2788,7 +2788,7 @@
         <v>178</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="D1" s="14" t="s">
         <v>166</v>
@@ -2817,7 +2817,7 @@
         <v>183</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="D2" s="15">
         <v>31005.82</v>
@@ -2842,7 +2842,7 @@
         <v>35</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="D3" s="15">
         <v>30704.52</v>
@@ -2888,7 +2888,7 @@
         <v>183</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="D5" s="15">
         <v>46695.85</v>
@@ -2907,11 +2907,11 @@
       <c r="A6" s="15">
         <v>5</v>
       </c>
-      <c r="B6" s="15" t="s">
-        <v>186</v>
+      <c r="B6" s="13" t="s">
+        <v>71</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="D6" s="15">
         <v>55065.36</v>
@@ -2932,11 +2932,11 @@
       <c r="A7" s="15">
         <v>6</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="13" t="s">
+        <v>213</v>
+      </c>
+      <c r="C7" s="13" t="s">
         <v>186</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>187</v>
       </c>
       <c r="D7" s="15">
         <v>6937.06</v>
@@ -2962,7 +2962,7 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2977,142 +2977,154 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="14" t="s">
         <v>177</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="14" t="s">
         <v>178</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>202</v>
-      </c>
-      <c r="D1" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="D1" s="14" t="s">
         <v>166</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="14" t="s">
         <v>172</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="14" t="s">
         <v>170</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="14" t="s">
         <v>154</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="14" t="s">
         <v>155</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="14" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="4">
+    <row r="2" spans="1:9" ht="185.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="16">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="17" t="s">
-        <v>213</v>
-      </c>
-      <c r="D2" s="4">
+      <c r="C2" s="13" t="s">
+        <v>219</v>
+      </c>
+      <c r="D2" s="16">
         <v>38711.08</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="16">
         <v>0</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="16" t="s">
         <v>181</v>
       </c>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
     </row>
     <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="4">
+      <c r="A3" s="16">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="16" t="s">
+        <v>187</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="D3" s="16">
+        <v>47724.32</v>
+      </c>
+      <c r="E3" s="16">
+        <v>47724.32</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>182</v>
+      </c>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="16">
+        <v>3</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" s="19"/>
+      <c r="D4" s="16">
+        <v>568.69000000000005</v>
+      </c>
+      <c r="E4" s="16">
+        <v>86.46</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+    </row>
+    <row r="5" spans="1:9" ht="131.44999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="16">
+        <v>4</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>212</v>
+      </c>
+      <c r="D5" s="16">
+        <v>2837.97</v>
+      </c>
+      <c r="E5" s="16">
+        <v>837</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" s="16" t="s">
         <v>188</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+    </row>
+    <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="16">
+        <v>5</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>211</v>
+      </c>
+      <c r="D6" s="16">
+        <v>35920.129999999997</v>
+      </c>
+      <c r="E6" s="16">
+        <v>5986.99</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="16" t="s">
         <v>189</v>
       </c>
-      <c r="D3" s="4">
-        <v>47724.32</v>
-      </c>
-      <c r="E3" s="4">
-        <v>47724.32</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="D4" s="4">
-        <v>568.69000000000005</v>
-      </c>
-      <c r="E4" s="4">
-        <v>86.46</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="131.44999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="4">
-        <v>4</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>221</v>
-      </c>
-      <c r="D5" s="4">
-        <v>2837.97</v>
-      </c>
-      <c r="E5" s="4">
-        <v>837</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="4">
-        <v>5</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="C6" s="17" t="s">
-        <v>220</v>
-      </c>
-      <c r="D6" s="4">
-        <v>35920.129999999997</v>
-      </c>
-      <c r="E6" s="4">
-        <v>5986.99</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>191</v>
-      </c>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3127,147 +3139,148 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" customWidth="1"/>
-    <col min="3" max="3" width="48.140625" customWidth="1"/>
-    <col min="4" max="6" width="20.140625" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" customWidth="1"/>
-    <col min="8" max="8" width="30" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" style="19" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" style="19" customWidth="1"/>
+    <col min="3" max="3" width="48.140625" style="19" customWidth="1"/>
+    <col min="4" max="6" width="20.140625" style="19" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" style="19" customWidth="1"/>
+    <col min="8" max="8" width="30" style="19" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" style="19" customWidth="1"/>
+    <col min="10" max="16384" width="12.7109375" style="19"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="14" t="s">
         <v>177</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="14" t="s">
         <v>178</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>202</v>
-      </c>
-      <c r="D1" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="D1" s="14" t="s">
         <v>166</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="14" t="s">
         <v>170</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="14" t="s">
         <v>154</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="14" t="s">
         <v>155</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="14" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="4">
+      <c r="A2" s="16">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="16" t="s">
+        <v>190</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>218</v>
+      </c>
+      <c r="D2" s="16">
+        <v>30897.62</v>
+      </c>
+      <c r="E2" s="20">
+        <v>30897.62</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="16">
+        <v>2</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" s="16">
+        <v>4589.6899999999996</v>
+      </c>
+      <c r="E3" s="16">
+        <v>458.69</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="16">
+        <v>3</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="C4" s="13" t="s">
         <v>192</v>
       </c>
-      <c r="C2" s="17" t="s">
-        <v>193</v>
-      </c>
-      <c r="D2" s="4">
-        <v>30897.62</v>
-      </c>
-      <c r="E2" s="10">
-        <v>30897.62</v>
-      </c>
-      <c r="F2" s="4" t="s">
+      <c r="D4" s="16">
+        <v>24614.37</v>
+      </c>
+      <c r="E4" s="16">
+        <v>0</v>
+      </c>
+      <c r="F4" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="4">
-        <v>2</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="D3" s="4">
-        <v>4589.6899999999996</v>
-      </c>
-      <c r="E3" s="4">
-        <v>458.69</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="C4" s="17" t="s">
-        <v>195</v>
-      </c>
-      <c r="D4" s="4">
-        <v>24614.37</v>
-      </c>
-      <c r="E4" s="4">
-        <v>0</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>26</v>
-      </c>
     </row>
     <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="4">
+      <c r="A5" s="16">
         <v>4</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="C5" s="17" t="s">
-        <v>214</v>
-      </c>
-      <c r="D5" s="4">
+      <c r="C5" s="13" t="s">
+        <v>208</v>
+      </c>
+      <c r="D5" s="16">
         <v>61067.12</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="16">
         <v>1067.02</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="16" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="4">
+      <c r="A6" s="16">
         <v>5</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="17" t="s">
-        <v>215</v>
-      </c>
-      <c r="D6" s="4">
+      <c r="C6" s="13" t="s">
+        <v>217</v>
+      </c>
+      <c r="D6" s="16">
         <v>142756.10999999999</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="16">
         <v>42598.66</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="16" t="s">
         <v>32</v>
       </c>
     </row>
@@ -3284,7 +3297,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3300,13 +3313,13 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
-        <v>196</v>
+        <v>177</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>178</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="D1" s="14" t="s">
         <v>166</v>
@@ -3329,14 +3342,14 @@
         <v>59</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>197</v>
+        <v>214</v>
       </c>
       <c r="D2" s="15">
         <v>29359.85</v>
       </c>
       <c r="E2" s="16"/>
       <c r="F2" s="15" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="G2" s="16"/>
     </row>
@@ -3348,7 +3361,7 @@
         <v>63</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D3" s="15">
         <v>21213.97</v>
@@ -3367,14 +3380,14 @@
         <v>30</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D4" s="15">
         <v>72272.429999999993</v>
       </c>
       <c r="E4" s="16"/>
       <c r="F4" s="15" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="G4" s="16"/>
     </row>
@@ -3881,7 +3894,7 @@
         <v>102</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="G4" s="4">
         <v>5</v>
@@ -3908,7 +3921,7 @@
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="H5" s="4">
         <v>369</v>
@@ -3956,7 +3969,7 @@
         <v>110</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="G7" s="4">
         <v>6.9</v>
@@ -4112,7 +4125,7 @@
         <v>102</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="G13" s="4">
         <v>6.6</v>
@@ -4170,7 +4183,7 @@
         <v>132</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="G15" s="4">
         <v>12</v>
@@ -4346,7 +4359,9 @@
   </sheetPr>
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>

<commit_message>
added item adjustment and accounts
</commit_message>
<xml_diff>
--- a/utils/GuidedKarobarData.xlsx
+++ b/utils/GuidedKarobarData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\VisualStudioProjects\Karobar_Revamp_Selenium\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99863323-7A68-4BBB-971B-1B7312ED70F6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A67E9232-2416-4EDD-8115-5D567DCC6117}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Overview" sheetId="1" r:id="rId1"/>
@@ -29,12 +29,12 @@
     <sheet name="Purchase Return Data" sheetId="14" r:id="rId14"/>
     <sheet name="Quotation Data" sheetId="15" r:id="rId15"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="225">
   <si>
     <t>Total To Receive</t>
   </si>
@@ -1024,12 +1024,24 @@
 2.80 @ Rs. 4555.45  
 Charge 1: Rs. 500.75  </t>
   </si>
+  <si>
+    <t>3,66,618.27</t>
+  </si>
+  <si>
+    <t>Party balance right after adding parties</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> After adding data</t>
+  </si>
+  <si>
+    <t>P&amp;L, closing stock right after adding item data</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1081,8 +1093,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1113,6 +1139,16 @@
         <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1123,10 +1159,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -1172,12 +1210,17 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="2" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1394,29 +1437,31 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="B1:Q33"/>
+  <dimension ref="B1:Q38"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="22.140625" customWidth="1"/>
-    <col min="6" max="6" width="19.85546875" customWidth="1"/>
-    <col min="7" max="8" width="14.28515625" customWidth="1"/>
-    <col min="10" max="10" width="20.140625" customWidth="1"/>
-    <col min="13" max="13" width="22.28515625" customWidth="1"/>
-    <col min="16" max="16" width="23.85546875" customWidth="1"/>
+    <col min="2" max="2" width="22.109375" customWidth="1"/>
+    <col min="6" max="6" width="19.88671875" customWidth="1"/>
+    <col min="7" max="8" width="14.33203125" customWidth="1"/>
+    <col min="10" max="10" width="20.109375" customWidth="1"/>
+    <col min="13" max="13" width="22.33203125" customWidth="1"/>
+    <col min="16" max="16" width="23.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="2:17" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="2:17" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
@@ -1435,7 +1480,7 @@
       <c r="I3" s="5"/>
       <c r="J3" s="6"/>
     </row>
-    <row r="4" spans="2:17" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
@@ -1452,7 +1497,7 @@
       <c r="I4" s="5"/>
       <c r="J4" s="6"/>
     </row>
-    <row r="5" spans="2:17" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
@@ -1471,7 +1516,7 @@
       <c r="I5" s="5"/>
       <c r="J5" s="6"/>
     </row>
-    <row r="6" spans="2:17" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="F6" s="2" t="s">
         <v>8</v>
       </c>
@@ -1482,31 +1527,31 @@
       <c r="I6" s="5"/>
       <c r="J6" s="6"/>
     </row>
-    <row r="12" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="21" t="s">
+    <row r="12" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22"/>
-      <c r="F12" s="21" t="s">
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
+      <c r="F12" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="G12" s="22"/>
+      <c r="G12" s="25"/>
       <c r="H12" s="9"/>
-      <c r="J12" s="21" t="s">
+      <c r="J12" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="K12" s="22"/>
-      <c r="M12" s="21" t="s">
+      <c r="K12" s="25"/>
+      <c r="M12" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="N12" s="22"/>
-      <c r="P12" s="21" t="s">
+      <c r="N12" s="25"/>
+      <c r="P12" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="Q12" s="22"/>
-    </row>
-    <row r="13" spans="2:17" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="Q12" s="25"/>
+    </row>
+    <row r="13" spans="2:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
         <v>14</v>
       </c>
@@ -1544,7 +1589,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="2:17" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="s">
         <v>23</v>
       </c>
@@ -1585,7 +1630,7 @@
         <v>5440.1</v>
       </c>
     </row>
-    <row r="15" spans="2:17" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
         <v>30</v>
       </c>
@@ -1623,7 +1668,7 @@
         <v>2420.34</v>
       </c>
     </row>
-    <row r="16" spans="2:17" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
         <v>35</v>
       </c>
@@ -1661,7 +1706,7 @@
         <v>8505.69</v>
       </c>
     </row>
-    <row r="17" spans="2:17" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
         <v>41</v>
       </c>
@@ -1699,7 +1744,7 @@
         <v>1519.05</v>
       </c>
     </row>
-    <row r="18" spans="2:17" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="s">
         <v>46</v>
       </c>
@@ -1725,7 +1770,7 @@
         <v>2914.94</v>
       </c>
     </row>
-    <row r="19" spans="2:17" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B19" s="4" t="s">
         <v>49</v>
       </c>
@@ -1746,7 +1791,7 @@
       </c>
       <c r="I19" s="7"/>
     </row>
-    <row r="20" spans="2:17" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B20" s="4" t="s">
         <v>51</v>
       </c>
@@ -1766,7 +1811,7 @@
         <v>4380.68</v>
       </c>
     </row>
-    <row r="21" spans="2:17" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
         <v>53</v>
       </c>
@@ -1786,7 +1831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:17" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
         <v>55</v>
       </c>
@@ -1806,7 +1851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:17" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B23" s="4" t="s">
         <v>57</v>
       </c>
@@ -1826,7 +1871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:17" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="s">
         <v>59</v>
       </c>
@@ -1846,7 +1891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="2:17" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B25" s="4" t="s">
         <v>61</v>
       </c>
@@ -1867,7 +1912,7 @@
       </c>
       <c r="I25" s="7"/>
     </row>
-    <row r="26" spans="2:17" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B26" s="4" t="s">
         <v>63</v>
       </c>
@@ -1887,7 +1932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:17" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="s">
         <v>65</v>
       </c>
@@ -1907,7 +1952,7 @@
         <v>873.99</v>
       </c>
     </row>
-    <row r="28" spans="2:17" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B28" s="4" t="s">
         <v>67</v>
       </c>
@@ -1927,7 +1972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:17" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
         <v>69</v>
       </c>
@@ -1947,7 +1992,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="2:17" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B30" s="4" t="s">
         <v>71</v>
       </c>
@@ -1967,7 +2012,7 @@
         <v>3729.12</v>
       </c>
     </row>
-    <row r="31" spans="2:17" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B31" s="4" t="s">
         <v>73</v>
       </c>
@@ -1987,7 +2032,7 @@
         <v>91791.45</v>
       </c>
     </row>
-    <row r="32" spans="2:17" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B32" s="4" t="s">
         <v>75</v>
       </c>
@@ -2007,7 +2052,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B33" s="4" t="s">
         <v>77</v>
       </c>
@@ -2027,13 +2072,41 @@
         <v>0</v>
       </c>
     </row>
+    <row r="36" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="24" t="s">
+        <v>223</v>
+      </c>
+      <c r="C36" s="24"/>
+      <c r="D36" s="24"/>
+    </row>
+    <row r="37" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="21" t="s">
+        <v>222</v>
+      </c>
+      <c r="C37" s="22">
+        <f>SUMIF('Party Data'!E2:E100, "Receivable", 'Party Data'!D2:D100)</f>
+        <v>3032.12</v>
+      </c>
+      <c r="D37" s="23">
+        <v>5553.48</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>224</v>
+      </c>
+      <c r="C38" t="s">
+        <v>221</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="P12:Q12"/>
+    <mergeCell ref="B36:D36"/>
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="F12:G12"/>
     <mergeCell ref="J12:K12"/>
     <mergeCell ref="M12:N12"/>
-    <mergeCell ref="P12:Q12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2046,20 +2119,22 @@
   </sheetPr>
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="20.140625" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="18.44140625" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" customWidth="1"/>
+    <col min="4" max="4" width="20.109375" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" customWidth="1"/>
     <col min="6" max="6" width="30" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>176</v>
       </c>
@@ -2082,7 +2157,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -2096,7 +2171,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -2110,7 +2185,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -2124,7 +2199,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -2138,7 +2213,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -2152,7 +2227,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -2166,7 +2241,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -2180,7 +2255,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -2194,7 +2269,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -2208,7 +2283,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -2238,18 +2313,18 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" customWidth="1"/>
-    <col min="3" max="3" width="48.140625" style="18" customWidth="1"/>
-    <col min="4" max="6" width="20.140625" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="18.44140625" customWidth="1"/>
+    <col min="3" max="3" width="48.109375" style="18" customWidth="1"/>
+    <col min="4" max="6" width="20.109375" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" customWidth="1"/>
     <col min="8" max="8" width="30" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" customWidth="1"/>
+    <col min="9" max="9" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:29" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>177</v>
       </c>
@@ -2298,7 +2373,7 @@
       <c r="AB1" s="12"/>
       <c r="AC1" s="12"/>
     </row>
-    <row r="2" spans="1:29" ht="28.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:29" ht="28.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13">
         <v>1</v>
       </c>
@@ -2341,7 +2416,7 @@
       <c r="AB2" s="12"/>
       <c r="AC2" s="12"/>
     </row>
-    <row r="3" spans="1:29" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:29" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13">
         <v>2</v>
       </c>
@@ -2382,7 +2457,7 @@
       <c r="AB3" s="12"/>
       <c r="AC3" s="12"/>
     </row>
-    <row r="4" spans="1:29" ht="90.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:29" ht="90.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13">
         <v>3</v>
       </c>
@@ -2425,7 +2500,7 @@
       <c r="AB4" s="12"/>
       <c r="AC4" s="12"/>
     </row>
-    <row r="5" spans="1:29" ht="237.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:29" ht="237.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13">
         <v>4</v>
       </c>
@@ -2468,7 +2543,7 @@
       <c r="AB5" s="12"/>
       <c r="AC5" s="12"/>
     </row>
-    <row r="6" spans="1:29" ht="64.900000000000006" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:29" ht="64.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13">
         <v>5</v>
       </c>
@@ -2511,7 +2586,7 @@
       <c r="AB6" s="12"/>
       <c r="AC6" s="12"/>
     </row>
-    <row r="7" spans="1:29" ht="161.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:29" ht="161.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13">
         <v>6</v>
       </c>
@@ -2554,7 +2629,7 @@
       <c r="AB7" s="12"/>
       <c r="AC7" s="12"/>
     </row>
-    <row r="8" spans="1:29" ht="141.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:29" ht="141.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13">
         <v>7</v>
       </c>
@@ -2599,7 +2674,7 @@
       <c r="AB8" s="12"/>
       <c r="AC8" s="12"/>
     </row>
-    <row r="9" spans="1:29" ht="205.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:29" ht="205.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13">
         <v>8</v>
       </c>
@@ -2644,7 +2719,7 @@
       <c r="AB9" s="12"/>
       <c r="AC9" s="12"/>
     </row>
-    <row r="10" spans="1:29" ht="216.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:29" ht="224.4" x14ac:dyDescent="0.25">
       <c r="A10" s="13">
         <v>9</v>
       </c>
@@ -2689,7 +2764,7 @@
       <c r="AB10" s="12"/>
       <c r="AC10" s="12"/>
     </row>
-    <row r="11" spans="1:29" ht="183" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:29" ht="183" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13">
         <v>10</v>
       </c>
@@ -2734,22 +2809,22 @@
       <c r="AB11" s="12"/>
       <c r="AC11" s="12"/>
     </row>
-    <row r="13" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="17"/>
     </row>
-    <row r="14" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="17"/>
     </row>
-    <row r="16" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C16" s="17"/>
     </row>
-    <row r="17" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C17" s="17"/>
     </row>
-    <row r="19" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C19" s="17"/>
     </row>
-    <row r="20" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C20" s="17"/>
     </row>
   </sheetData>
@@ -2769,18 +2844,18 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" customWidth="1"/>
-    <col min="3" max="3" width="48.140625" customWidth="1"/>
-    <col min="4" max="6" width="20.140625" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="18.44140625" customWidth="1"/>
+    <col min="3" max="3" width="48.109375" customWidth="1"/>
+    <col min="4" max="6" width="20.109375" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" customWidth="1"/>
     <col min="8" max="8" width="30" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" customWidth="1"/>
+    <col min="9" max="9" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>177</v>
       </c>
@@ -2809,7 +2884,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15">
         <v>1</v>
       </c>
@@ -2834,7 +2909,7 @@
       <c r="H2" s="16"/>
       <c r="I2" s="16"/>
     </row>
-    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15">
         <v>2</v>
       </c>
@@ -2859,7 +2934,7 @@
       <c r="H3" s="16"/>
       <c r="I3" s="16"/>
     </row>
-    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15">
         <v>3</v>
       </c>
@@ -2880,7 +2955,7 @@
       <c r="H4" s="16"/>
       <c r="I4" s="16"/>
     </row>
-    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15">
         <v>4</v>
       </c>
@@ -2903,7 +2978,7 @@
       <c r="H5" s="16"/>
       <c r="I5" s="16"/>
     </row>
-    <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="15">
         <v>5</v>
       </c>
@@ -2928,7 +3003,7 @@
       <c r="H6" s="16"/>
       <c r="I6" s="16"/>
     </row>
-    <row r="7" spans="1:9" ht="409.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="409.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="15">
         <v>6</v>
       </c>
@@ -2948,7 +3023,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2965,18 +3040,18 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" customWidth="1"/>
-    <col min="3" max="3" width="48.140625" customWidth="1"/>
-    <col min="4" max="6" width="20.140625" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="18.44140625" customWidth="1"/>
+    <col min="3" max="3" width="48.109375" customWidth="1"/>
+    <col min="4" max="6" width="20.109375" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" customWidth="1"/>
     <col min="8" max="8" width="30" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" customWidth="1"/>
+    <col min="9" max="9" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>177</v>
       </c>
@@ -3005,7 +3080,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="185.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="185.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="16">
         <v>1</v>
       </c>
@@ -3030,7 +3105,7 @@
       <c r="H2" s="19"/>
       <c r="I2" s="19"/>
     </row>
-    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="16">
         <v>2</v>
       </c>
@@ -3055,7 +3130,7 @@
       <c r="H3" s="19"/>
       <c r="I3" s="19"/>
     </row>
-    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16">
         <v>3</v>
       </c>
@@ -3076,7 +3151,7 @@
       <c r="H4" s="19"/>
       <c r="I4" s="19"/>
     </row>
-    <row r="5" spans="1:9" ht="131.44999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="131.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="16">
         <v>4</v>
       </c>
@@ -3101,7 +3176,7 @@
       <c r="H5" s="19"/>
       <c r="I5" s="19"/>
     </row>
-    <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="16">
         <v>5</v>
       </c>
@@ -3142,19 +3217,19 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" style="19" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" style="19" customWidth="1"/>
-    <col min="3" max="3" width="48.140625" style="19" customWidth="1"/>
-    <col min="4" max="6" width="20.140625" style="19" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" style="19" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" style="19" customWidth="1"/>
+    <col min="2" max="2" width="18.44140625" style="19" customWidth="1"/>
+    <col min="3" max="3" width="48.109375" style="19" customWidth="1"/>
+    <col min="4" max="6" width="20.109375" style="19" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" style="19" customWidth="1"/>
     <col min="8" max="8" width="30" style="19" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" style="19" customWidth="1"/>
-    <col min="10" max="16384" width="12.7109375" style="19"/>
+    <col min="9" max="9" width="14.6640625" style="19" customWidth="1"/>
+    <col min="10" max="16384" width="12.6640625" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>177</v>
       </c>
@@ -3183,7 +3258,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="16">
         <v>1</v>
       </c>
@@ -3207,7 +3282,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="16">
         <v>2</v>
       </c>
@@ -3224,7 +3299,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16">
         <v>3</v>
       </c>
@@ -3244,7 +3319,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="16">
         <v>4</v>
       </c>
@@ -3264,7 +3339,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="16">
         <v>5</v>
       </c>
@@ -3300,18 +3375,18 @@
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" customWidth="1"/>
-    <col min="3" max="3" width="48.140625" customWidth="1"/>
-    <col min="4" max="4" width="20.140625" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="18.44140625" customWidth="1"/>
+    <col min="3" max="3" width="48.109375" customWidth="1"/>
+    <col min="4" max="4" width="20.109375" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" customWidth="1"/>
     <col min="6" max="6" width="30" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>177</v>
       </c>
@@ -3334,7 +3409,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15">
         <v>1</v>
       </c>
@@ -3353,7 +3428,7 @@
       </c>
       <c r="G2" s="16"/>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15">
         <v>2</v>
       </c>
@@ -3372,7 +3447,7 @@
       </c>
       <c r="G3" s="16"/>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15">
         <v>3</v>
       </c>
@@ -3404,18 +3479,18 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>14</v>
       </c>
@@ -3432,7 +3507,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>23</v>
       </c>
@@ -3449,7 +3524,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>30</v>
       </c>
@@ -3466,7 +3541,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>35</v>
       </c>
@@ -3483,7 +3558,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>41</v>
       </c>
@@ -3500,7 +3575,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>46</v>
       </c>
@@ -3517,7 +3592,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>49</v>
       </c>
@@ -3534,7 +3609,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>51</v>
       </c>
@@ -3551,7 +3626,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>53</v>
       </c>
@@ -3568,7 +3643,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>55</v>
       </c>
@@ -3585,7 +3660,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>57</v>
       </c>
@@ -3602,7 +3677,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>59</v>
       </c>
@@ -3619,7 +3694,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>61</v>
       </c>
@@ -3636,7 +3711,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>63</v>
       </c>
@@ -3653,7 +3728,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>65</v>
       </c>
@@ -3670,7 +3745,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>67</v>
       </c>
@@ -3687,7 +3762,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>69</v>
       </c>
@@ -3704,7 +3779,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>71</v>
       </c>
@@ -3721,7 +3796,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>73</v>
       </c>
@@ -3738,7 +3813,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>75</v>
       </c>
@@ -3755,7 +3830,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>77</v>
       </c>
@@ -3785,21 +3860,22 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="7" width="14.7109375" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" customWidth="1"/>
+    <col min="5" max="7" width="14.6640625" customWidth="1"/>
+    <col min="8" max="8" width="16.44140625" customWidth="1"/>
     <col min="9" max="10" width="19" customWidth="1"/>
+    <col min="11" max="11" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>17</v>
       </c>
@@ -3831,7 +3907,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>25</v>
       </c>
@@ -3854,7 +3930,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>31</v>
       </c>
@@ -3877,7 +3953,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>37</v>
       </c>
@@ -3909,7 +3985,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>42</v>
       </c>
@@ -3933,7 +4009,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>47</v>
       </c>
@@ -3952,7 +4028,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>50</v>
       </c>
@@ -3984,7 +4060,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>52</v>
       </c>
@@ -4010,7 +4086,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>54</v>
       </c>
@@ -4042,7 +4118,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>56</v>
       </c>
@@ -4063,7 +4139,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>58</v>
       </c>
@@ -4089,7 +4165,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>60</v>
       </c>
@@ -4108,7 +4184,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>62</v>
       </c>
@@ -4140,7 +4216,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>64</v>
       </c>
@@ -4166,7 +4242,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>130</v>
       </c>
@@ -4198,7 +4274,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>68</v>
       </c>
@@ -4224,7 +4300,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>70</v>
       </c>
@@ -4243,7 +4319,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>72</v>
       </c>
@@ -4273,7 +4349,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>74</v>
       </c>
@@ -4296,7 +4372,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>76</v>
       </c>
@@ -4315,7 +4391,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>78</v>
       </c>
@@ -4359,21 +4435,22 @@
   </sheetPr>
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="14.7109375" customWidth="1"/>
-    <col min="3" max="3" width="21.28515625" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" customWidth="1"/>
+    <col min="3" max="3" width="21.33203125" customWidth="1"/>
+    <col min="4" max="4" width="21.6640625" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" customWidth="1"/>
+    <col min="6" max="6" width="17.6640625" customWidth="1"/>
     <col min="7" max="7" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>150</v>
       </c>
@@ -4396,7 +4473,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>156</v>
       </c>
@@ -4410,7 +4487,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>157</v>
       </c>
@@ -4427,7 +4504,7 @@
         <v>45.69</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>156</v>
       </c>
@@ -4441,7 +4518,7 @@
         <v>69.400000000000006</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>157</v>
       </c>
@@ -4455,7 +4532,7 @@
         <v>566.54999999999995</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>156</v>
       </c>
@@ -4469,7 +4546,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>157</v>
       </c>
@@ -4486,7 +4563,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>156</v>
       </c>
@@ -4500,7 +4577,7 @@
         <v>65.98</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>157</v>
       </c>
@@ -4514,7 +4591,7 @@
         <v>32.33</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>156</v>
       </c>
@@ -4531,7 +4608,7 @@
         <v>635.9</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>157</v>
       </c>
@@ -4548,7 +4625,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>156</v>
       </c>
@@ -4565,7 +4642,7 @@
         <v>1220</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>157</v>
       </c>
@@ -4582,7 +4659,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>156</v>
       </c>
@@ -4599,7 +4676,7 @@
         <v>98.45</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>157</v>
       </c>
@@ -4616,7 +4693,7 @@
         <v>875.9</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>156</v>
       </c>
@@ -4630,7 +4707,7 @@
         <v>452.96</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>157</v>
       </c>
@@ -4647,7 +4724,7 @@
         <v>365.9</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>156</v>
       </c>
@@ -4664,7 +4741,7 @@
         <v>425.3</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>157</v>
       </c>
@@ -4681,7 +4758,7 @@
         <v>690.6</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>156</v>
       </c>
@@ -4698,7 +4775,7 @@
         <v>120.93</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>157</v>
       </c>
@@ -4727,14 +4804,16 @@
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>20</v>
       </c>
@@ -4742,7 +4821,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>26</v>
       </c>
@@ -4750,7 +4829,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>32</v>
       </c>
@@ -4758,7 +4837,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>38</v>
       </c>
@@ -4766,7 +4845,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>43</v>
       </c>
@@ -4788,17 +4867,17 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
-    <col min="2" max="2" width="21.28515625" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" customWidth="1"/>
-    <col min="5" max="5" width="20.140625" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="21.33203125" customWidth="1"/>
+    <col min="3" max="3" width="18.44140625" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" customWidth="1"/>
+    <col min="5" max="5" width="20.109375" customWidth="1"/>
     <col min="6" max="6" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>163</v>
       </c>
@@ -4818,7 +4897,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>156</v>
       </c>
@@ -4829,7 +4908,7 @@
         <v>4560</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>157</v>
       </c>
@@ -4840,7 +4919,7 @@
         <v>56.36</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>167</v>
       </c>
@@ -4854,7 +4933,7 @@
         <v>214.98</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>156</v>
       </c>
@@ -4865,7 +4944,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>167</v>
       </c>
@@ -4879,7 +4958,7 @@
         <v>123.6</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>157</v>
       </c>
@@ -4890,7 +4969,7 @@
         <v>5699.6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>156</v>
       </c>
@@ -4901,7 +4980,7 @@
         <v>458.5</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>167</v>
       </c>
@@ -4915,7 +4994,7 @@
         <v>12.66</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>156</v>
       </c>
@@ -4926,7 +5005,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>157</v>
       </c>
@@ -4937,7 +5016,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>157</v>
       </c>
@@ -4948,7 +5027,7 @@
         <v>535.36</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>156</v>
       </c>
@@ -4971,20 +5050,22 @@
   </sheetPr>
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="20.140625" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="18.44140625" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" customWidth="1"/>
+    <col min="4" max="4" width="20.109375" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" customWidth="1"/>
     <col min="6" max="6" width="30" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>168</v>
       </c>
@@ -5007,7 +5088,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -5021,7 +5102,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -5035,7 +5116,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -5049,7 +5130,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -5063,7 +5144,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -5077,7 +5158,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -5091,7 +5172,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -5105,7 +5186,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -5119,7 +5200,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -5133,7 +5214,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -5147,7 +5228,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -5161,7 +5242,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -5175,7 +5256,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -5189,7 +5270,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -5203,7 +5284,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -5217,7 +5298,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -5231,7 +5312,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>17</v>
       </c>
@@ -5245,7 +5326,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>18</v>
       </c>
@@ -5259,7 +5340,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>19</v>
       </c>
@@ -5273,7 +5354,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>20</v>
       </c>
@@ -5301,18 +5382,18 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="20.140625" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="18.44140625" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" customWidth="1"/>
+    <col min="4" max="4" width="20.109375" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" customWidth="1"/>
     <col min="6" max="6" width="30" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>168</v>
       </c>
@@ -5335,7 +5416,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -5349,7 +5430,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -5363,7 +5444,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -5377,7 +5458,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -5391,7 +5472,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -5405,7 +5486,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -5419,7 +5500,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -5433,7 +5514,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -5447,7 +5528,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -5464,7 +5545,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -5478,7 +5559,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -5492,7 +5573,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -5506,7 +5587,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -5520,7 +5601,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -5534,7 +5615,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -5548,7 +5629,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -5562,7 +5643,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>17</v>
       </c>
@@ -5576,7 +5657,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>18</v>
       </c>
@@ -5590,7 +5671,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>19</v>
       </c>
@@ -5604,7 +5685,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>20</v>
       </c>
@@ -5632,18 +5713,18 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="20.140625" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="18.44140625" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" customWidth="1"/>
+    <col min="4" max="4" width="20.109375" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" customWidth="1"/>
     <col min="6" max="6" width="30" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>173</v>
       </c>
@@ -5666,7 +5747,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -5680,7 +5761,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -5694,7 +5775,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -5708,7 +5789,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -5722,7 +5803,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -5736,7 +5817,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -5750,7 +5831,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -5764,7 +5845,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -5778,7 +5859,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -5792,7 +5873,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -5806,7 +5887,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -5820,7 +5901,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
added payment in out methods and ddt from excel
</commit_message>
<xml_diff>
--- a/utils/GuidedKarobarData.xlsx
+++ b/utils/GuidedKarobarData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\VisualStudioProjects\Karobar_Revamp_Selenium\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A67E9232-2416-4EDD-8115-5D567DCC6117}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51D435D0-1294-4B94-A58A-C947F0B776AD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Overview" sheetId="1" r:id="rId1"/>
@@ -19,8 +19,8 @@
     <sheet name="Item Adjustment Data" sheetId="4" r:id="rId4"/>
     <sheet name="Bank Accounts Data" sheetId="5" r:id="rId5"/>
     <sheet name="Transaction Adjustment Data" sheetId="6" r:id="rId6"/>
-    <sheet name="Payments In Data" sheetId="7" r:id="rId7"/>
-    <sheet name="Payments Out Data" sheetId="8" r:id="rId8"/>
+    <sheet name="Payments Out Data" sheetId="8" r:id="rId7"/>
+    <sheet name="Payments In Data" sheetId="7" r:id="rId8"/>
     <sheet name="Expenses Data" sheetId="9" r:id="rId9"/>
     <sheet name="Other Income Data" sheetId="10" r:id="rId10"/>
     <sheet name="Sales Data" sheetId="11" r:id="rId11"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="232">
   <si>
     <t>Total To Receive</t>
   </si>
@@ -1028,13 +1028,38 @@
     <t>3,66,618.27</t>
   </si>
   <si>
-    <t>Party balance right after adding parties</t>
-  </si>
-  <si>
     <t xml:space="preserve"> After adding data</t>
   </si>
   <si>
     <t>P&amp;L, closing stock right after adding item data</t>
+  </si>
+  <si>
+    <t>Account adjustments</t>
+  </si>
+  <si>
+    <t>Cash: -1583.58
+eSewa: -297.86
+NMB: 643.64
+Nabil: 3310.94</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Party balance right after adding parties. To receive and to give from dashboard</t>
+  </si>
+  <si>
+    <t>After payment in, dashboard to give and to receive</t>
+  </si>
+  <si>
+    <t>3,99,476.28</t>
+  </si>
+  <si>
+    <t>P&amp;L closing stock after item adjustment are added</t>
+  </si>
+  <si>
+    <t>Manage Account: 
+Cash: +5563.45, NMB: +1974.05, NABIL: +18925.63, eSewa:  +1328.5</t>
   </si>
 </sst>
 </file>
@@ -1164,7 +1189,7 @@
     <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -1211,12 +1236,15 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="2" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="8" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="9" fillId="7" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="8" fillId="6" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="9" fillId="7" borderId="0" xfId="2" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -1437,31 +1465,32 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="B1:Q38"/>
+  <dimension ref="B1:Q41"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="22.109375" customWidth="1"/>
-    <col min="6" max="6" width="19.88671875" customWidth="1"/>
-    <col min="7" max="8" width="14.33203125" customWidth="1"/>
-    <col min="10" max="10" width="20.109375" customWidth="1"/>
-    <col min="13" max="13" width="22.33203125" customWidth="1"/>
-    <col min="16" max="16" width="23.88671875" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" customWidth="1"/>
+    <col min="7" max="8" width="14.28515625" customWidth="1"/>
+    <col min="10" max="10" width="20.140625" customWidth="1"/>
+    <col min="13" max="13" width="22.28515625" customWidth="1"/>
+    <col min="16" max="16" width="23.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="2:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="2:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
@@ -1480,7 +1509,7 @@
       <c r="I3" s="5"/>
       <c r="J3" s="6"/>
     </row>
-    <row r="4" spans="2:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
@@ -1497,7 +1526,7 @@
       <c r="I4" s="5"/>
       <c r="J4" s="6"/>
     </row>
-    <row r="5" spans="2:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
@@ -1516,7 +1545,7 @@
       <c r="I5" s="5"/>
       <c r="J5" s="6"/>
     </row>
-    <row r="6" spans="2:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F6" s="2" t="s">
         <v>8</v>
       </c>
@@ -1527,31 +1556,31 @@
       <c r="I6" s="5"/>
       <c r="J6" s="6"/>
     </row>
-    <row r="12" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="24" t="s">
+    <row r="12" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="F12" s="24" t="s">
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="F12" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="G12" s="25"/>
+      <c r="G12" s="24"/>
       <c r="H12" s="9"/>
-      <c r="J12" s="24" t="s">
+      <c r="J12" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="K12" s="25"/>
-      <c r="M12" s="24" t="s">
+      <c r="K12" s="24"/>
+      <c r="M12" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="N12" s="25"/>
-      <c r="P12" s="24" t="s">
+      <c r="N12" s="24"/>
+      <c r="P12" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="Q12" s="25"/>
-    </row>
-    <row r="13" spans="2:17" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="Q12" s="24"/>
+    </row>
+    <row r="13" spans="2:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B13" s="3" t="s">
         <v>14</v>
       </c>
@@ -1589,7 +1618,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="2:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B14" s="4" t="s">
         <v>23</v>
       </c>
@@ -1630,7 +1659,7 @@
         <v>5440.1</v>
       </c>
     </row>
-    <row r="15" spans="2:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B15" s="4" t="s">
         <v>30</v>
       </c>
@@ -1668,7 +1697,7 @@
         <v>2420.34</v>
       </c>
     </row>
-    <row r="16" spans="2:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B16" s="4" t="s">
         <v>35</v>
       </c>
@@ -1706,7 +1735,7 @@
         <v>8505.69</v>
       </c>
     </row>
-    <row r="17" spans="2:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B17" s="4" t="s">
         <v>41</v>
       </c>
@@ -1744,7 +1773,7 @@
         <v>1519.05</v>
       </c>
     </row>
-    <row r="18" spans="2:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B18" s="4" t="s">
         <v>46</v>
       </c>
@@ -1770,7 +1799,7 @@
         <v>2914.94</v>
       </c>
     </row>
-    <row r="19" spans="2:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B19" s="4" t="s">
         <v>49</v>
       </c>
@@ -1791,7 +1820,7 @@
       </c>
       <c r="I19" s="7"/>
     </row>
-    <row r="20" spans="2:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B20" s="4" t="s">
         <v>51</v>
       </c>
@@ -1811,7 +1840,7 @@
         <v>4380.68</v>
       </c>
     </row>
-    <row r="21" spans="2:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B21" s="4" t="s">
         <v>53</v>
       </c>
@@ -1831,7 +1860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B22" s="4" t="s">
         <v>55</v>
       </c>
@@ -1851,7 +1880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B23" s="4" t="s">
         <v>57</v>
       </c>
@@ -1871,7 +1900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B24" s="4" t="s">
         <v>59</v>
       </c>
@@ -1891,7 +1920,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="2:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B25" s="4" t="s">
         <v>61</v>
       </c>
@@ -1912,7 +1941,7 @@
       </c>
       <c r="I25" s="7"/>
     </row>
-    <row r="26" spans="2:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B26" s="4" t="s">
         <v>63</v>
       </c>
@@ -1932,7 +1961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B27" s="4" t="s">
         <v>65</v>
       </c>
@@ -1952,7 +1981,7 @@
         <v>873.99</v>
       </c>
     </row>
-    <row r="28" spans="2:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B28" s="4" t="s">
         <v>67</v>
       </c>
@@ -1972,7 +2001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B29" s="4" t="s">
         <v>69</v>
       </c>
@@ -1992,7 +2021,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="2:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B30" s="4" t="s">
         <v>71</v>
       </c>
@@ -2012,7 +2041,7 @@
         <v>3729.12</v>
       </c>
     </row>
-    <row r="31" spans="2:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B31" s="4" t="s">
         <v>73</v>
       </c>
@@ -2032,7 +2061,7 @@
         <v>91791.45</v>
       </c>
     </row>
-    <row r="32" spans="2:17" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B32" s="4" t="s">
         <v>75</v>
       </c>
@@ -2052,7 +2081,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B33" s="4" t="s">
         <v>77</v>
       </c>
@@ -2072,31 +2101,61 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="24" t="s">
-        <v>223</v>
-      </c>
-      <c r="C36" s="24"/>
-      <c r="D36" s="24"/>
-    </row>
-    <row r="37" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="23" t="s">
+        <v>222</v>
+      </c>
+      <c r="C36" s="23"/>
+      <c r="D36" s="23"/>
+    </row>
+    <row r="37" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="21" t="s">
-        <v>222</v>
-      </c>
-      <c r="C37" s="22">
+        <v>227</v>
+      </c>
+      <c r="C37" s="25">
         <f>SUMIF('Party Data'!E2:E100, "Receivable", 'Party Data'!D2:D100)</f>
         <v>3032.12</v>
       </c>
-      <c r="D37" s="23">
+      <c r="D37" s="26">
         <v>5553.48</v>
       </c>
     </row>
-    <row r="38" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C38" t="s">
         <v>221</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" s="22" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B39" s="22" t="s">
+        <v>230</v>
+      </c>
+      <c r="C39" s="22" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B40" t="s">
+        <v>224</v>
+      </c>
+      <c r="C40" s="18" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B41" t="s">
+        <v>228</v>
+      </c>
+      <c r="C41" s="27">
+        <v>1146.95</v>
+      </c>
+      <c r="D41" s="28">
+        <v>31459.49</v>
+      </c>
+      <c r="E41" s="18" t="s">
+        <v>231</v>
       </c>
     </row>
   </sheetData>
@@ -2123,18 +2182,18 @@
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" customWidth="1"/>
-    <col min="2" max="2" width="18.44140625" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="20.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
     <col min="6" max="6" width="30" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>176</v>
       </c>
@@ -2157,7 +2216,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -2171,7 +2230,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -2185,7 +2244,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -2199,7 +2258,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -2213,7 +2272,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -2227,7 +2286,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -2241,7 +2300,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -2255,7 +2314,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -2269,7 +2328,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -2283,7 +2342,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -2309,22 +2368,22 @@
   </sheetPr>
   <dimension ref="A1:AC20"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" customWidth="1"/>
-    <col min="2" max="2" width="18.44140625" customWidth="1"/>
-    <col min="3" max="3" width="48.109375" style="18" customWidth="1"/>
-    <col min="4" max="6" width="20.109375" customWidth="1"/>
-    <col min="7" max="7" width="16.33203125" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="48.140625" style="18" customWidth="1"/>
+    <col min="4" max="6" width="20.140625" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" customWidth="1"/>
     <col min="8" max="8" width="30" customWidth="1"/>
-    <col min="9" max="9" width="14.6640625" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>177</v>
       </c>
@@ -2373,7 +2432,7 @@
       <c r="AB1" s="12"/>
       <c r="AC1" s="12"/>
     </row>
-    <row r="2" spans="1:29" ht="28.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" ht="28.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="13">
         <v>1</v>
       </c>
@@ -2416,7 +2475,7 @@
       <c r="AB2" s="12"/>
       <c r="AC2" s="12"/>
     </row>
-    <row r="3" spans="1:29" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="13">
         <v>2</v>
       </c>
@@ -2457,7 +2516,7 @@
       <c r="AB3" s="12"/>
       <c r="AC3" s="12"/>
     </row>
-    <row r="4" spans="1:29" ht="90.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" ht="90.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="13">
         <v>3</v>
       </c>
@@ -2500,7 +2559,7 @@
       <c r="AB4" s="12"/>
       <c r="AC4" s="12"/>
     </row>
-    <row r="5" spans="1:29" ht="237.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" ht="237.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="13">
         <v>4</v>
       </c>
@@ -2543,7 +2602,7 @@
       <c r="AB5" s="12"/>
       <c r="AC5" s="12"/>
     </row>
-    <row r="6" spans="1:29" ht="64.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" ht="64.900000000000006" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="13">
         <v>5</v>
       </c>
@@ -2586,7 +2645,7 @@
       <c r="AB6" s="12"/>
       <c r="AC6" s="12"/>
     </row>
-    <row r="7" spans="1:29" ht="161.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" ht="161.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="13">
         <v>6</v>
       </c>
@@ -2629,7 +2688,7 @@
       <c r="AB7" s="12"/>
       <c r="AC7" s="12"/>
     </row>
-    <row r="8" spans="1:29" ht="141.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" ht="141.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="13">
         <v>7</v>
       </c>
@@ -2674,7 +2733,7 @@
       <c r="AB8" s="12"/>
       <c r="AC8" s="12"/>
     </row>
-    <row r="9" spans="1:29" ht="205.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" ht="205.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="13">
         <v>8</v>
       </c>
@@ -2719,7 +2778,7 @@
       <c r="AB9" s="12"/>
       <c r="AC9" s="12"/>
     </row>
-    <row r="10" spans="1:29" ht="224.4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29" ht="216.75" x14ac:dyDescent="0.2">
       <c r="A10" s="13">
         <v>9</v>
       </c>
@@ -2764,7 +2823,7 @@
       <c r="AB10" s="12"/>
       <c r="AC10" s="12"/>
     </row>
-    <row r="11" spans="1:29" ht="183" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29" ht="183" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="13">
         <v>10</v>
       </c>
@@ -2809,22 +2868,22 @@
       <c r="AB11" s="12"/>
       <c r="AC11" s="12"/>
     </row>
-    <row r="13" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C13" s="17"/>
     </row>
-    <row r="14" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C14" s="17"/>
     </row>
-    <row r="16" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C16" s="17"/>
     </row>
-    <row r="17" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C17" s="17"/>
     </row>
-    <row r="19" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C19" s="17"/>
     </row>
-    <row r="20" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C20" s="17"/>
     </row>
   </sheetData>
@@ -2841,21 +2900,21 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" customWidth="1"/>
-    <col min="2" max="2" width="18.44140625" customWidth="1"/>
-    <col min="3" max="3" width="48.109375" customWidth="1"/>
-    <col min="4" max="6" width="20.109375" customWidth="1"/>
-    <col min="7" max="7" width="16.33203125" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="48.140625" customWidth="1"/>
+    <col min="4" max="6" width="20.140625" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" customWidth="1"/>
     <col min="8" max="8" width="30" customWidth="1"/>
-    <col min="9" max="9" width="14.6640625" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
         <v>177</v>
       </c>
@@ -2884,7 +2943,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="15">
         <v>1</v>
       </c>
@@ -2909,7 +2968,7 @@
       <c r="H2" s="16"/>
       <c r="I2" s="16"/>
     </row>
-    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="15">
         <v>2</v>
       </c>
@@ -2934,7 +2993,7 @@
       <c r="H3" s="16"/>
       <c r="I3" s="16"/>
     </row>
-    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="15">
         <v>3</v>
       </c>
@@ -2955,7 +3014,7 @@
       <c r="H4" s="16"/>
       <c r="I4" s="16"/>
     </row>
-    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="15">
         <v>4</v>
       </c>
@@ -2978,7 +3037,7 @@
       <c r="H5" s="16"/>
       <c r="I5" s="16"/>
     </row>
-    <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="15">
         <v>5</v>
       </c>
@@ -3003,7 +3062,7 @@
       <c r="H6" s="16"/>
       <c r="I6" s="16"/>
     </row>
-    <row r="7" spans="1:9" ht="409.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="409.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="15">
         <v>6</v>
       </c>
@@ -3023,7 +3082,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3040,18 +3099,18 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" customWidth="1"/>
-    <col min="2" max="2" width="18.44140625" customWidth="1"/>
-    <col min="3" max="3" width="48.109375" customWidth="1"/>
-    <col min="4" max="6" width="20.109375" customWidth="1"/>
-    <col min="7" max="7" width="16.33203125" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="48.140625" customWidth="1"/>
+    <col min="4" max="6" width="20.140625" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" customWidth="1"/>
     <col min="8" max="8" width="30" customWidth="1"/>
-    <col min="9" max="9" width="14.6640625" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
         <v>177</v>
       </c>
@@ -3080,7 +3139,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="185.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="185.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="16">
         <v>1</v>
       </c>
@@ -3105,7 +3164,7 @@
       <c r="H2" s="19"/>
       <c r="I2" s="19"/>
     </row>
-    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="16">
         <v>2</v>
       </c>
@@ -3130,7 +3189,7 @@
       <c r="H3" s="19"/>
       <c r="I3" s="19"/>
     </row>
-    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16">
         <v>3</v>
       </c>
@@ -3151,7 +3210,7 @@
       <c r="H4" s="19"/>
       <c r="I4" s="19"/>
     </row>
-    <row r="5" spans="1:9" ht="131.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="131.44999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="16">
         <v>4</v>
       </c>
@@ -3176,7 +3235,7 @@
       <c r="H5" s="19"/>
       <c r="I5" s="19"/>
     </row>
-    <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="16">
         <v>5</v>
       </c>
@@ -3217,19 +3276,19 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" style="19" customWidth="1"/>
-    <col min="2" max="2" width="18.44140625" style="19" customWidth="1"/>
-    <col min="3" max="3" width="48.109375" style="19" customWidth="1"/>
-    <col min="4" max="6" width="20.109375" style="19" customWidth="1"/>
-    <col min="7" max="7" width="16.33203125" style="19" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" style="19" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" style="19" customWidth="1"/>
+    <col min="3" max="3" width="48.140625" style="19" customWidth="1"/>
+    <col min="4" max="6" width="20.140625" style="19" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" style="19" customWidth="1"/>
     <col min="8" max="8" width="30" style="19" customWidth="1"/>
-    <col min="9" max="9" width="14.6640625" style="19" customWidth="1"/>
-    <col min="10" max="16384" width="12.6640625" style="19"/>
+    <col min="9" max="9" width="14.7109375" style="19" customWidth="1"/>
+    <col min="10" max="16384" width="12.7109375" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
         <v>177</v>
       </c>
@@ -3258,7 +3317,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="16">
         <v>1</v>
       </c>
@@ -3282,7 +3341,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="16">
         <v>2</v>
       </c>
@@ -3299,7 +3358,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16">
         <v>3</v>
       </c>
@@ -3319,7 +3378,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="16">
         <v>4</v>
       </c>
@@ -3339,7 +3398,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="16">
         <v>5</v>
       </c>
@@ -3375,18 +3434,18 @@
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" customWidth="1"/>
-    <col min="2" max="2" width="18.44140625" customWidth="1"/>
-    <col min="3" max="3" width="48.109375" customWidth="1"/>
-    <col min="4" max="4" width="20.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="48.140625" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
     <col min="6" max="6" width="30" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
         <v>177</v>
       </c>
@@ -3409,7 +3468,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="15">
         <v>1</v>
       </c>
@@ -3428,7 +3487,7 @@
       </c>
       <c r="G2" s="16"/>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="15">
         <v>2</v>
       </c>
@@ -3447,7 +3506,7 @@
       </c>
       <c r="G3" s="16"/>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="15">
         <v>3</v>
       </c>
@@ -3482,15 +3541,15 @@
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>14</v>
       </c>
@@ -3507,7 +3566,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>23</v>
       </c>
@@ -3524,7 +3583,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>30</v>
       </c>
@@ -3541,7 +3600,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>35</v>
       </c>
@@ -3558,7 +3617,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>41</v>
       </c>
@@ -3575,7 +3634,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>46</v>
       </c>
@@ -3592,7 +3651,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>49</v>
       </c>
@@ -3609,7 +3668,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>51</v>
       </c>
@@ -3626,7 +3685,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>53</v>
       </c>
@@ -3643,7 +3702,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>55</v>
       </c>
@@ -3660,7 +3719,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>57</v>
       </c>
@@ -3677,7 +3736,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>59</v>
       </c>
@@ -3694,7 +3753,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>61</v>
       </c>
@@ -3711,7 +3770,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>63</v>
       </c>
@@ -3728,7 +3787,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>65</v>
       </c>
@@ -3745,7 +3804,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>67</v>
       </c>
@@ -3762,7 +3821,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>69</v>
       </c>
@@ -3779,7 +3838,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>71</v>
       </c>
@@ -3796,7 +3855,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>73</v>
       </c>
@@ -3813,7 +3872,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>75</v>
       </c>
@@ -3830,7 +3889,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>77</v>
       </c>
@@ -3860,22 +3919,22 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="7" width="14.6640625" customWidth="1"/>
-    <col min="8" max="8" width="16.44140625" customWidth="1"/>
+    <col min="5" max="7" width="14.7109375" customWidth="1"/>
+    <col min="8" max="8" width="16.42578125" customWidth="1"/>
     <col min="9" max="10" width="19" customWidth="1"/>
-    <col min="11" max="11" width="17.33203125" customWidth="1"/>
+    <col min="11" max="11" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>17</v>
       </c>
@@ -3907,7 +3966,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>25</v>
       </c>
@@ -3930,7 +3989,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>31</v>
       </c>
@@ -3953,7 +4012,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>37</v>
       </c>
@@ -3985,7 +4044,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>42</v>
       </c>
@@ -4009,7 +4068,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>47</v>
       </c>
@@ -4028,7 +4087,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>50</v>
       </c>
@@ -4060,7 +4119,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>52</v>
       </c>
@@ -4086,7 +4145,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>54</v>
       </c>
@@ -4118,7 +4177,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>56</v>
       </c>
@@ -4139,7 +4198,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>58</v>
       </c>
@@ -4165,7 +4224,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>60</v>
       </c>
@@ -4184,7 +4243,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>62</v>
       </c>
@@ -4216,7 +4275,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>64</v>
       </c>
@@ -4242,7 +4301,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>130</v>
       </c>
@@ -4274,7 +4333,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>68</v>
       </c>
@@ -4300,7 +4359,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>70</v>
       </c>
@@ -4319,7 +4378,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>72</v>
       </c>
@@ -4349,7 +4408,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>74</v>
       </c>
@@ -4372,7 +4431,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>76</v>
       </c>
@@ -4391,7 +4450,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>78</v>
       </c>
@@ -4439,18 +4498,18 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" customWidth="1"/>
-    <col min="3" max="3" width="21.33203125" customWidth="1"/>
-    <col min="4" max="4" width="21.6640625" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="21.28515625" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" customWidth="1"/>
     <col min="7" max="7" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>150</v>
       </c>
@@ -4473,7 +4532,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>156</v>
       </c>
@@ -4487,7 +4546,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>157</v>
       </c>
@@ -4504,7 +4563,7 @@
         <v>45.69</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>156</v>
       </c>
@@ -4518,7 +4577,7 @@
         <v>69.400000000000006</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>157</v>
       </c>
@@ -4532,7 +4591,7 @@
         <v>566.54999999999995</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>156</v>
       </c>
@@ -4546,7 +4605,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>157</v>
       </c>
@@ -4563,7 +4622,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>156</v>
       </c>
@@ -4577,7 +4636,7 @@
         <v>65.98</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>157</v>
       </c>
@@ -4591,7 +4650,7 @@
         <v>32.33</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>156</v>
       </c>
@@ -4608,7 +4667,7 @@
         <v>635.9</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>157</v>
       </c>
@@ -4625,7 +4684,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>156</v>
       </c>
@@ -4642,7 +4701,7 @@
         <v>1220</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>157</v>
       </c>
@@ -4659,7 +4718,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>156</v>
       </c>
@@ -4676,7 +4735,7 @@
         <v>98.45</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>157</v>
       </c>
@@ -4693,7 +4752,7 @@
         <v>875.9</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>156</v>
       </c>
@@ -4707,7 +4766,7 @@
         <v>452.96</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>157</v>
       </c>
@@ -4724,7 +4783,7 @@
         <v>365.9</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>156</v>
       </c>
@@ -4741,7 +4800,7 @@
         <v>425.3</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>157</v>
       </c>
@@ -4758,7 +4817,7 @@
         <v>690.6</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>156</v>
       </c>
@@ -4775,7 +4834,7 @@
         <v>120.93</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>157</v>
       </c>
@@ -4804,16 +4863,16 @@
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>20</v>
       </c>
@@ -4821,7 +4880,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>26</v>
       </c>
@@ -4829,7 +4888,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>32</v>
       </c>
@@ -4837,7 +4896,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>38</v>
       </c>
@@ -4845,7 +4904,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>43</v>
       </c>
@@ -4865,19 +4924,21 @@
   </sheetPr>
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" customWidth="1"/>
-    <col min="2" max="2" width="21.33203125" customWidth="1"/>
-    <col min="3" max="3" width="18.44140625" customWidth="1"/>
-    <col min="4" max="4" width="15.6640625" customWidth="1"/>
-    <col min="5" max="5" width="20.109375" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="21.28515625" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" customWidth="1"/>
     <col min="6" max="6" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>163</v>
       </c>
@@ -4897,7 +4958,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>156</v>
       </c>
@@ -4908,7 +4969,7 @@
         <v>4560</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>157</v>
       </c>
@@ -4919,7 +4980,7 @@
         <v>56.36</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>167</v>
       </c>
@@ -4933,7 +4994,7 @@
         <v>214.98</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>156</v>
       </c>
@@ -4944,7 +5005,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>167</v>
       </c>
@@ -4958,7 +5019,7 @@
         <v>123.6</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>157</v>
       </c>
@@ -4969,7 +5030,7 @@
         <v>5699.6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>156</v>
       </c>
@@ -4980,7 +5041,7 @@
         <v>458.5</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>167</v>
       </c>
@@ -4994,7 +5055,7 @@
         <v>12.66</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>156</v>
       </c>
@@ -5005,7 +5066,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>157</v>
       </c>
@@ -5016,7 +5077,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>157</v>
       </c>
@@ -5027,7 +5088,7 @@
         <v>535.36</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>156</v>
       </c>
@@ -5044,28 +5105,361 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:G21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
+    <col min="6" max="6" width="30" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="4">
+        <v>800</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="4">
+        <v>546.69000000000005</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" s="4">
+        <v>123.88</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" s="4">
+        <v>5000</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" s="4">
+        <v>596.6</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="4">
+        <v>6</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" s="4">
+        <v>785</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="4">
+        <v>7</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" s="4">
+        <v>255</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="4">
+        <v>8</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" s="4">
+        <v>999</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="4">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="4">
+        <v>888.66</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="4">
+        <v>10</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C11" s="4">
+        <v>256.68</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="4">
+        <v>11</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" s="4">
+        <v>123.89</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="4">
+        <v>12</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" s="4">
+        <v>90</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="4">
+        <v>13</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" s="4">
+        <v>3000</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="4">
+        <v>14</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" s="4">
+        <v>5000</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="4">
+        <v>15</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="4">
+        <v>4569.6000000000004</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="4">
+        <v>16</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="4">
+        <v>700</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="4">
+        <v>17</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="4">
+        <v>900</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="4">
+        <v>18</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="4">
+        <v>456.6</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="4">
+        <v>19</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C20" s="4">
+        <v>985</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="4">
+        <v>20</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C21" s="4">
+        <v>98.89</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView zoomScale="102" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" customWidth="1"/>
-    <col min="2" max="2" width="18.44140625" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="20.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
     <col min="6" max="6" width="30" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>168</v>
       </c>
@@ -5073,7 +5467,7 @@
         <v>14</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>169</v>
+        <v>226</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>170</v>
@@ -5088,7 +5482,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -5102,7 +5496,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -5116,7 +5510,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -5130,7 +5524,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -5144,7 +5538,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -5158,7 +5552,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -5172,7 +5566,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -5186,7 +5580,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -5200,7 +5594,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -5214,7 +5608,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -5228,7 +5622,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -5242,7 +5636,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -5256,7 +5650,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -5270,7 +5664,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -5284,7 +5678,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -5298,7 +5692,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -5312,7 +5706,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
         <v>17</v>
       </c>
@@ -5326,7 +5720,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4">
         <v>18</v>
       </c>
@@ -5340,7 +5734,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
         <v>19</v>
       </c>
@@ -5354,7 +5748,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
         <v>20</v>
       </c>
@@ -5363,337 +5757,6 @@
       </c>
       <c r="C21" s="4">
         <v>69.64</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="A1:G21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14.6640625" customWidth="1"/>
-    <col min="2" max="2" width="18.44140625" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="20.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" customWidth="1"/>
-    <col min="6" max="6" width="30" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C2" s="4">
-        <v>800</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
-        <v>2</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="C3" s="4">
-        <v>546.69000000000005</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="C4" s="4">
-        <v>123.88</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
-        <v>4</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="C5" s="4">
-        <v>5000</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
-        <v>5</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C6" s="4">
-        <v>596.6</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
-        <v>6</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="C7" s="4">
-        <v>785</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
-        <v>7</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="C8" s="4">
-        <v>255</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
-        <v>8</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="C9" s="4">
-        <v>999</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
-        <v>9</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C10" s="4">
-        <v>888.66</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
-        <v>10</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="C11" s="4">
-        <v>256.68</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
-        <v>11</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="C12" s="4">
-        <v>123.89</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
-        <v>12</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="C13" s="4">
-        <v>90</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="4">
-        <v>13</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="C14" s="4">
-        <v>3000</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="4">
-        <v>14</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="C15" s="4">
-        <v>5000</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="4">
-        <v>15</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16" s="4">
-        <v>4569.6000000000004</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="4">
-        <v>16</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C17" s="4">
-        <v>700</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="4">
-        <v>17</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="C18" s="4">
-        <v>900</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="4">
-        <v>18</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="C19" s="4">
-        <v>456.6</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="4">
-        <v>19</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="C20" s="4">
-        <v>985</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="4">
-        <v>20</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="C21" s="4">
-        <v>98.89</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>38</v>
@@ -5713,18 +5776,18 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" customWidth="1"/>
-    <col min="2" max="2" width="18.44140625" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="20.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
     <col min="6" max="6" width="30" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>173</v>
       </c>
@@ -5747,7 +5810,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -5761,7 +5824,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -5775,7 +5838,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -5789,7 +5852,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -5803,7 +5866,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -5817,7 +5880,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -5831,7 +5894,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -5845,7 +5908,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -5859,7 +5922,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -5873,7 +5936,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -5887,7 +5950,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -5901,7 +5964,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
added income expense flow and some twerks
</commit_message>
<xml_diff>
--- a/utils/GuidedKarobarData.xlsx
+++ b/utils/GuidedKarobarData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\VisualStudioProjects\Karobar_Revamp_Selenium\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51D435D0-1294-4B94-A58A-C947F0B776AD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51EEF9DF-09F5-42AF-9736-5F6485309333}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,10 +19,10 @@
     <sheet name="Item Adjustment Data" sheetId="4" r:id="rId4"/>
     <sheet name="Bank Accounts Data" sheetId="5" r:id="rId5"/>
     <sheet name="Transaction Adjustment Data" sheetId="6" r:id="rId6"/>
-    <sheet name="Payments Out Data" sheetId="8" r:id="rId7"/>
-    <sheet name="Payments In Data" sheetId="7" r:id="rId8"/>
-    <sheet name="Expenses Data" sheetId="9" r:id="rId9"/>
-    <sheet name="Other Income Data" sheetId="10" r:id="rId10"/>
+    <sheet name="Payments In Data" sheetId="7" r:id="rId7"/>
+    <sheet name="Payments Out Data" sheetId="8" r:id="rId8"/>
+    <sheet name="Other Income Data" sheetId="10" r:id="rId9"/>
+    <sheet name="Expenses Data" sheetId="9" r:id="rId10"/>
     <sheet name="Sales Data" sheetId="11" r:id="rId11"/>
     <sheet name="Purchase Data" sheetId="12" r:id="rId12"/>
     <sheet name="Sales Return Data" sheetId="13" r:id="rId13"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="233">
   <si>
     <t>Total To Receive</t>
   </si>
@@ -558,16 +558,7 @@
     <t>Paid Amount</t>
   </si>
   <si>
-    <t>Expense Number</t>
-  </si>
-  <si>
     <t>Category</t>
-  </si>
-  <si>
-    <t>Travel</t>
-  </si>
-  <si>
-    <t>Income Number</t>
   </si>
   <si>
     <t>Invoice No.</t>
@@ -897,21 +888,6 @@
 Charge 2: Rs. 600.67</t>
   </si>
   <si>
-    <t>Billing Items:
-Item 3:  
-9.20 BOX @ Rs. 880.30  
-Item 6:  
-8.10 CAN @ Rs. 369.55  
-Item 10:  
-7.75 BOX @ Rs. 986.75  
-Item 14:  
-5.45 BAGS @ Rs. 458.99  
-Item 20:  
-10.80 BOX @ Rs. 955.99  
-Tax: 13%  
-Charge 1: Rs. 250.98</t>
-  </si>
-  <si>
     <t xml:space="preserve">Billing Items:
 Item 2:  
 4.65 @ Rs. 120.50  
@@ -935,20 +911,6 @@
 8.25 BOX @ Rs. 986.30  
 Tax: 13%  
 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Billing Items:
-Item 1:  
-7.30 @ Rs. 650.45  
-Item 4:  
-18.40 PCS @ Rs. 369.99  
-Item 14:  
-5.50 BAGS @ Rs. 458.99  
-Item 20:  
-6.85 BOX @ Rs. 955.99  
-Overall Discount: 10.50%  
-Tax: 13%  
-Charge 1: Rs. 350.75  </t>
   </si>
   <si>
     <t xml:space="preserve">Billing Items:
@@ -1058,8 +1020,51 @@
     <t>P&amp;L closing stock after item adjustment are added</t>
   </si>
   <si>
+    <t>After payment out, dashboard to give and to receive</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
     <t>Manage Account: 
-Cash: +5563.45, NMB: +1974.05, NABIL: +18925.63, eSewa:  +1328.5</t>
+Cash: +3979.87, eSewa: +1030.64, NMB: +2617.69, Nabil:  +22236.57</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manage Account: 
+Cash: +2610.99,
+eSewa: -4330.31, NMB: -10850.8, NABIL: +16259.4 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Billing Items:
+Item 1:  
+7.30 @ Rs. 650.45  
+Item 4:  
+18.40 PCS @ Rs. 369.99  
+Item 14:  
+5.50 BAG @ Rs. 458.99  
+Item 20:  
+6.85 BOX @ Rs. 955.99  
+Overall Discount: 10.50%  
+Tax: 13%  
+Charge 1: Rs. 350.75  </t>
+  </si>
+  <si>
+    <t>Billing Items:
+Item 3:  
+9.20 BOX @ Rs. 880.30  
+Item 6:  
+8.10 CAN @ Rs. 369.55  
+Item 10:  
+7.75 BOX @ Rs. 986.75  
+Item 14:  
+5.45 BAG @ Rs. 458.99  
+Item 20:  
+10.80 BOX @ Rs. 955.99  
+Tax: 13%  
+Charge 1: Rs. 250.98</t>
+  </si>
+  <si>
+    <t>Travel &amp; Transportation</t>
   </si>
 </sst>
 </file>
@@ -1189,7 +1194,7 @@
     <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -1237,14 +1242,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="8" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="9" fillId="7" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="8" fillId="6" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="9" fillId="7" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -1465,10 +1471,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="B1:Q41"/>
+  <dimension ref="B1:Q42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1557,28 +1563,28 @@
       <c r="J6" s="6"/>
     </row>
     <row r="12" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
-      <c r="F12" s="23" t="s">
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="F12" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="G12" s="24"/>
+      <c r="G12" s="29"/>
       <c r="H12" s="9"/>
-      <c r="J12" s="23" t="s">
+      <c r="J12" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="K12" s="24"/>
-      <c r="M12" s="23" t="s">
+      <c r="K12" s="29"/>
+      <c r="M12" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="N12" s="24"/>
-      <c r="P12" s="23" t="s">
+      <c r="N12" s="29"/>
+      <c r="P12" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="Q12" s="24"/>
+      <c r="Q12" s="29"/>
     </row>
     <row r="13" spans="2:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B13" s="3" t="s">
@@ -2102,60 +2108,74 @@
       </c>
     </row>
     <row r="36" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="23" t="s">
-        <v>222</v>
-      </c>
-      <c r="C36" s="23"/>
-      <c r="D36" s="23"/>
+      <c r="B36" s="28" t="s">
+        <v>217</v>
+      </c>
+      <c r="C36" s="28"/>
+      <c r="D36" s="28"/>
     </row>
     <row r="37" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="21" t="s">
-        <v>227</v>
-      </c>
-      <c r="C37" s="25">
+        <v>222</v>
+      </c>
+      <c r="C37" s="24">
         <f>SUMIF('Party Data'!E2:E100, "Receivable", 'Party Data'!D2:D100)</f>
         <v>3032.12</v>
       </c>
-      <c r="D37" s="26">
+      <c r="D37" s="25">
         <v>5553.48</v>
       </c>
     </row>
     <row r="38" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="C38" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
     </row>
     <row r="39" spans="2:8" s="22" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="22" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="C39" s="22" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
     </row>
     <row r="40" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="C40" s="18" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
     </row>
     <row r="41" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
+        <v>223</v>
+      </c>
+      <c r="C41" s="26">
+        <v>1146.95</v>
+      </c>
+      <c r="D41" s="27">
+        <v>31459.49</v>
+      </c>
+      <c r="E41" s="18" t="s">
         <v>228</v>
       </c>
-      <c r="C41" s="27">
-        <v>1146.95</v>
-      </c>
-      <c r="D41" s="28">
-        <v>31459.49</v>
-      </c>
-      <c r="E41" s="18" t="s">
-        <v>231</v>
+    </row>
+    <row r="42" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B42" s="23" t="s">
+        <v>226</v>
+      </c>
+      <c r="C42" s="26">
+        <v>14818.33</v>
+      </c>
+      <c r="D42" s="27">
+        <v>18955.830000000002</v>
+      </c>
+      <c r="E42" s="18" t="s">
+        <v>229</v>
       </c>
     </row>
   </sheetData>
@@ -2172,14 +2192,14 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2195,10 +2215,10 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>176</v>
+        <v>227</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>166</v>
@@ -2221,10 +2241,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>29</v>
+        <v>232</v>
       </c>
       <c r="C2" s="4">
-        <v>4560.6000000000004</v>
+        <v>5860</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>32</v>
@@ -2235,10 +2255,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C3" s="4">
-        <v>235.69</v>
+        <v>453</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>26</v>
@@ -2249,10 +2269,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="C4" s="4">
-        <v>7845</v>
+        <v>658.65</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>38</v>
@@ -2263,13 +2283,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C5" s="4">
-        <v>562.6</v>
+        <v>1256</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2277,13 +2297,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C6" s="4">
-        <v>78.599999999999994</v>
+        <v>2365.66</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2291,10 +2311,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>34</v>
+        <v>232</v>
       </c>
       <c r="C7" s="4">
-        <v>984.65</v>
+        <v>1250</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>38</v>
@@ -2305,13 +2325,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C8" s="4">
-        <v>1200</v>
+        <v>452</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2319,13 +2339,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C9" s="4">
-        <v>660.69</v>
+        <v>365.69</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2333,13 +2353,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C10" s="4">
-        <v>956.45</v>
+        <v>1256.3</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2347,13 +2367,41 @@
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C11" s="4">
-        <v>800.9</v>
+        <v>780</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>32</v>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="4">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="C12" s="4">
+        <v>980</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="4">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" s="4">
+        <v>999.99</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -2368,8 +2416,8 @@
   </sheetPr>
   <dimension ref="A1:AC20"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2385,13 +2433,13 @@
   <sheetData>
     <row r="1" spans="1:29" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>166</v>
@@ -2437,10 +2485,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D2" s="13">
         <v>2670</v>
@@ -2524,7 +2572,7 @@
         <v>53</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D4" s="13">
         <v>38510.400000000001</v>
@@ -2567,7 +2615,7 @@
         <v>46</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D5" s="13">
         <v>1928.92</v>
@@ -2610,7 +2658,7 @@
         <v>77</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D6" s="13">
         <v>18023.169999999998</v>
@@ -2653,7 +2701,7 @@
         <v>73</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D7" s="13">
         <v>52252.06</v>
@@ -2696,7 +2744,7 @@
         <v>75</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="D8" s="13">
         <v>565320.32999999996</v>
@@ -2708,7 +2756,7 @@
         <v>32</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="H8" s="12"/>
       <c r="I8" s="12"/>
@@ -2741,7 +2789,7 @@
         <v>59</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="D9" s="13">
         <v>125453.23</v>
@@ -2753,7 +2801,7 @@
         <v>43</v>
       </c>
       <c r="G9" s="13" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="H9" s="12"/>
       <c r="I9" s="12"/>
@@ -2783,10 +2831,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D10" s="13">
         <v>77212</v>
@@ -2798,7 +2846,7 @@
         <v>26</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="H10" s="12"/>
       <c r="I10" s="12"/>
@@ -2831,7 +2879,7 @@
         <v>41</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D11" s="13">
         <v>28846.5</v>
@@ -2843,7 +2891,7 @@
         <v>38</v>
       </c>
       <c r="G11" s="13" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="H11" s="12"/>
       <c r="I11" s="12"/>
@@ -2899,7 +2947,7 @@
   </sheetPr>
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -2916,13 +2964,13 @@
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D1" s="14" t="s">
         <v>166</v>
@@ -2948,10 +2996,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="D2" s="15">
         <v>31005.82</v>
@@ -2963,7 +3011,7 @@
         <v>26</v>
       </c>
       <c r="G2" s="15" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="H2" s="16"/>
       <c r="I2" s="16"/>
@@ -2976,7 +3024,7 @@
         <v>35</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="D3" s="15">
         <v>30704.52</v>
@@ -2988,7 +3036,7 @@
         <v>43</v>
       </c>
       <c r="G3" s="15" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="H3" s="16"/>
       <c r="I3" s="16"/>
@@ -3019,10 +3067,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D5" s="15">
         <v>46695.85</v>
@@ -3045,7 +3093,7 @@
         <v>71</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D6" s="15">
         <v>55065.36</v>
@@ -3057,7 +3105,7 @@
         <v>32</v>
       </c>
       <c r="G6" s="15" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="H6" s="16"/>
       <c r="I6" s="16"/>
@@ -3067,10 +3115,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D7" s="15">
         <v>6937.06</v>
@@ -3095,8 +3143,8 @@
   </sheetPr>
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3112,13 +3160,13 @@
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D1" s="14" t="s">
         <v>166</v>
@@ -3147,7 +3195,7 @@
         <v>35</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="D2" s="16">
         <v>38711.08</v>
@@ -3159,7 +3207,7 @@
         <v>32</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="H2" s="19"/>
       <c r="I2" s="19"/>
@@ -3169,10 +3217,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="D3" s="16">
         <v>47724.32</v>
@@ -3184,7 +3232,7 @@
         <v>26</v>
       </c>
       <c r="G3" s="16" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="H3" s="19"/>
       <c r="I3" s="19"/>
@@ -3218,7 +3266,7 @@
         <v>75</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="D5" s="16">
         <v>2837.97</v>
@@ -3230,7 +3278,7 @@
         <v>43</v>
       </c>
       <c r="G5" s="16" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="H5" s="19"/>
       <c r="I5" s="19"/>
@@ -3243,7 +3291,7 @@
         <v>73</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>211</v>
+        <v>231</v>
       </c>
       <c r="D6" s="16">
         <v>35920.129999999997</v>
@@ -3255,7 +3303,7 @@
         <v>26</v>
       </c>
       <c r="G6" s="16" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="H6" s="19"/>
       <c r="I6" s="19"/>
@@ -3273,7 +3321,7 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3290,13 +3338,13 @@
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D1" s="14" t="s">
         <v>166</v>
@@ -3322,10 +3370,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="D2" s="16">
         <v>30897.62</v>
@@ -3338,7 +3386,7 @@
       </c>
       <c r="G2" s="16"/>
       <c r="H2" s="16" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3366,7 +3414,7 @@
         <v>73</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="D4" s="16">
         <v>24614.37</v>
@@ -3386,7 +3434,7 @@
         <v>69</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D5" s="16">
         <v>61067.12</v>
@@ -3406,7 +3454,7 @@
         <v>30</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="D6" s="16">
         <v>142756.10999999999</v>
@@ -3431,7 +3479,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3447,13 +3495,13 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D1" s="14" t="s">
         <v>166</v>
@@ -3476,14 +3524,14 @@
         <v>59</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="D2" s="15">
         <v>29359.85</v>
       </c>
       <c r="E2" s="16"/>
       <c r="F2" s="15" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G2" s="16"/>
     </row>
@@ -3495,14 +3543,14 @@
         <v>63</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>215</v>
+        <v>230</v>
       </c>
       <c r="D3" s="15">
         <v>21213.97</v>
       </c>
       <c r="E3" s="16"/>
       <c r="F3" s="15" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="G3" s="16"/>
     </row>
@@ -3514,14 +3562,14 @@
         <v>30</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="D4" s="15">
         <v>72272.429999999993</v>
       </c>
       <c r="E4" s="16"/>
       <c r="F4" s="15" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="G4" s="16"/>
     </row>
@@ -3918,8 +3966,8 @@
   </sheetPr>
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4029,7 +4077,7 @@
         <v>102</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G4" s="4">
         <v>5</v>
@@ -4056,7 +4104,7 @@
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="H5" s="4">
         <v>369</v>
@@ -4104,7 +4152,7 @@
         <v>110</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="G7" s="4">
         <v>6.9</v>
@@ -4260,7 +4308,7 @@
         <v>102</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G13" s="4">
         <v>6.6</v>
@@ -4318,7 +4366,7 @@
         <v>132</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G15" s="4">
         <v>12</v>
@@ -4495,7 +4543,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4925,7 +4973,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5105,14 +5153,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView zoomScale="102" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5134,7 +5182,7 @@
         <v>14</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>170</v>
@@ -5154,13 +5202,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>49</v>
+        <v>23</v>
       </c>
       <c r="C2" s="4">
-        <v>800</v>
+        <v>500</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5168,13 +5216,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C3" s="4">
-        <v>546.69000000000005</v>
+        <v>65.650000000000006</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5182,10 +5230,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>77</v>
+        <v>46</v>
       </c>
       <c r="C4" s="4">
-        <v>123.88</v>
+        <v>123.54</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>26</v>
@@ -5196,13 +5244,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="C5" s="4">
-        <v>5000</v>
+        <v>8999</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5210,13 +5258,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C6" s="4">
-        <v>596.6</v>
+        <v>960.36</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5224,13 +5272,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="C7" s="4">
-        <v>785</v>
+        <v>456.36</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5238,10 +5286,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="C8" s="4">
-        <v>255</v>
+        <v>259.45</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>26</v>
@@ -5252,13 +5300,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C9" s="4">
-        <v>999</v>
+        <v>780</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5266,16 +5314,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C10" s="4">
-        <v>888.66</v>
+        <v>563</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>32</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5283,13 +5328,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C11" s="4">
-        <v>256.68</v>
+        <v>210.6</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5300,7 +5345,7 @@
         <v>59</v>
       </c>
       <c r="C12" s="4">
-        <v>123.89</v>
+        <v>9850</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>43</v>
@@ -5311,10 +5356,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="C13" s="4">
-        <v>90</v>
+        <v>78.599999999999994</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>26</v>
@@ -5325,13 +5370,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="C14" s="4">
-        <v>3000</v>
+        <v>4566</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5342,7 +5387,7 @@
         <v>49</v>
       </c>
       <c r="C15" s="4">
-        <v>5000</v>
+        <v>20.03</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>43</v>
@@ -5353,10 +5398,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="C16" s="4">
-        <v>4569.6000000000004</v>
+        <v>98.4</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>38</v>
@@ -5367,13 +5412,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="C17" s="4">
-        <v>700</v>
+        <v>56.6</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5381,10 +5426,10 @@
         <v>17</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>46</v>
+        <v>73</v>
       </c>
       <c r="C18" s="4">
-        <v>900</v>
+        <v>79.5</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>26</v>
@@ -5395,10 +5440,10 @@
         <v>18</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>41</v>
+        <v>69</v>
       </c>
       <c r="C19" s="4">
-        <v>456.6</v>
+        <v>42.3</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>32</v>
@@ -5409,10 +5454,10 @@
         <v>19</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C20" s="4">
-        <v>985</v>
+        <v>12.6</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>32</v>
@@ -5423,10 +5468,10 @@
         <v>20</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C21" s="4">
-        <v>98.89</v>
+        <v>69.64</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>38</v>
@@ -5438,14 +5483,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView zoomScale="102" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5467,7 +5512,7 @@
         <v>14</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>170</v>
@@ -5487,13 +5532,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="C2" s="4">
-        <v>500</v>
+        <v>800</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5501,13 +5546,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="C3" s="4">
-        <v>65.650000000000006</v>
+        <v>546.69000000000005</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5515,10 +5560,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
       <c r="C4" s="4">
-        <v>123.54</v>
+        <v>123.88</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>26</v>
@@ -5529,13 +5574,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="C5" s="4">
-        <v>8999</v>
+        <v>5000</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5543,13 +5588,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="C6" s="4">
-        <v>960.36</v>
+        <v>596.6</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5557,13 +5602,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="C7" s="4">
-        <v>456.36</v>
+        <v>785</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5571,10 +5616,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="C8" s="4">
-        <v>259.45</v>
+        <v>255</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>26</v>
@@ -5585,13 +5630,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C9" s="4">
-        <v>780</v>
+        <v>999</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5599,13 +5644,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C10" s="4">
-        <v>563</v>
+        <v>888.66</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>32</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5613,13 +5661,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C11" s="4">
-        <v>210.6</v>
+        <v>256.68</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5630,7 +5678,7 @@
         <v>59</v>
       </c>
       <c r="C12" s="4">
-        <v>9850</v>
+        <v>123.89</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>43</v>
@@ -5641,10 +5689,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="C13" s="4">
-        <v>78.599999999999994</v>
+        <v>90</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>26</v>
@@ -5655,13 +5703,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="C14" s="4">
-        <v>4566</v>
+        <v>3000</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5672,7 +5720,7 @@
         <v>49</v>
       </c>
       <c r="C15" s="4">
-        <v>20.03</v>
+        <v>5000</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>43</v>
@@ -5683,10 +5731,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>49</v>
+        <v>23</v>
       </c>
       <c r="C16" s="4">
-        <v>98.4</v>
+        <v>4569.6000000000004</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>38</v>
@@ -5697,13 +5745,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="C17" s="4">
-        <v>56.6</v>
+        <v>700</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5711,10 +5759,10 @@
         <v>17</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>73</v>
+        <v>46</v>
       </c>
       <c r="C18" s="4">
-        <v>79.5</v>
+        <v>900</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>26</v>
@@ -5725,10 +5773,10 @@
         <v>18</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>69</v>
+        <v>41</v>
       </c>
       <c r="C19" s="4">
-        <v>42.3</v>
+        <v>456.6</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>32</v>
@@ -5739,10 +5787,10 @@
         <v>19</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="C20" s="4">
-        <v>12.6</v>
+        <v>985</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>32</v>
@@ -5753,10 +5801,10 @@
         <v>20</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="C21" s="4">
-        <v>69.64</v>
+        <v>98.89</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>38</v>
@@ -5768,13 +5816,15 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -5789,10 +5839,10 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>173</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>174</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>166</v>
@@ -5815,10 +5865,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>175</v>
+        <v>29</v>
       </c>
       <c r="C2" s="4">
-        <v>5860</v>
+        <v>4560.6000000000004</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>32</v>
@@ -5829,10 +5879,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C3" s="4">
-        <v>453</v>
+        <v>235.69</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>26</v>
@@ -5843,10 +5893,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C4" s="4">
-        <v>658.65</v>
+        <v>7845</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>38</v>
@@ -5857,13 +5907,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="C5" s="4">
-        <v>1256</v>
+        <v>562.6</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5871,13 +5921,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C6" s="4">
-        <v>2365.66</v>
+        <v>78.599999999999994</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5885,10 +5935,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>175</v>
+        <v>34</v>
       </c>
       <c r="C7" s="4">
-        <v>1250</v>
+        <v>984.65</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>38</v>
@@ -5899,13 +5949,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C8" s="4">
-        <v>452</v>
+        <v>1200</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5913,13 +5963,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C9" s="4">
-        <v>365.69</v>
+        <v>660.69</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5927,13 +5977,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C10" s="4">
-        <v>1256.3</v>
+        <v>956.45</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5941,41 +5991,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C11" s="4">
-        <v>780</v>
+        <v>800.9</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="4">
-        <v>11</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="C12" s="4">
-        <v>980</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="4">
-        <v>12</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C13" s="4">
-        <v>999.99</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>